<commit_message>
Invigilation Step 3 & 4 done.
</commit_message>
<xml_diff>
--- a/backend/media/temp/ExamDateSheet.xlsx
+++ b/backend/media/temp/ExamDateSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\8th Sem\IP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E456D29-0151-47B5-B23D-4B79689E6512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A40A48-34E3-471D-B5B6-16AC8D5E3301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -57,9 +57,6 @@
     <t>BDMH</t>
   </si>
   <si>
-    <t>CV</t>
-  </si>
-  <si>
     <t>WCE</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>VPM</t>
   </si>
   <si>
-    <t>BIO543</t>
-  </si>
-  <si>
     <t>CSE344/CSE544/ ECE344/ECE544</t>
   </si>
   <si>
@@ -93,33 +87,21 @@
     <t>PSY302</t>
   </si>
   <si>
-    <t xml:space="preserve">MTH310/MTH520 </t>
-  </si>
-  <si>
     <t>MTH372</t>
   </si>
   <si>
     <t>CSE573</t>
   </si>
   <si>
-    <t>ECO332</t>
-  </si>
-  <si>
     <t>C101,LHC</t>
   </si>
   <si>
-    <t>C201,LHC</t>
-  </si>
-  <si>
     <t>C03,Old Acad</t>
   </si>
   <si>
     <t>C02,Old Acad</t>
   </si>
   <si>
-    <t>C21,Old Acad</t>
-  </si>
-  <si>
     <t>C12,Old Acad</t>
   </si>
   <si>
@@ -133,6 +115,27 @@
   </si>
   <si>
     <t>DES512</t>
+  </si>
+  <si>
+    <t>C2001,LHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BIO543</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MTH310 / MTH520      </t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,8 +623,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="16">
-        <v>45413</v>
+      <c r="A2" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -633,13 +636,13 @@
         <v>9</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="F2" s="6">
         <v>127</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -652,17 +655,15 @@
       <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="6">
         <v>109</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -673,19 +674,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="6">
         <v>3</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -699,16 +700,14 @@
         <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="6">
-        <v>21</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -722,39 +721,37 @@
         <v>8</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="6">
         <v>33</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>45413</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F7" s="6">
         <v>18</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -768,16 +765,16 @@
         <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F8" s="6">
         <v>84</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -791,21 +788,21 @@
         <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9" s="6">
         <v>39</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
-        <v>45413</v>
+        <v>45414</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -814,16 +811,16 @@
         <v>8</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F10" s="13">
         <v>185</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>